<commit_message>
#phuc.nguyen Connect Account Stripe
</commit_message>
<xml_diff>
--- a/docs/HuuPhuc/Manager Company 1.xlsx
+++ b/docs/HuuPhuc/Manager Company 1.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83AD1094-54D0-42FB-8A12-1104AF3641C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{307A209E-8A2A-4190-A43D-38B23C722CD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="7" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All My Company" sheetId="1" r:id="rId1"/>
     <sheet name="Create Company" sheetId="2" r:id="rId2"/>
-    <sheet name="Check Company Account " sheetId="5" r:id="rId3"/>
-    <sheet name="My Company" sheetId="6" r:id="rId4"/>
-    <sheet name="List DeletedCompany" sheetId="9" r:id="rId5"/>
-    <sheet name="Update Company" sheetId="12" r:id="rId6"/>
-    <sheet name="Create Compan" sheetId="13" r:id="rId7"/>
-    <sheet name="Detail Company" sheetId="10" r:id="rId8"/>
-    <sheet name="Group of CompanyID" sheetId="11" r:id="rId9"/>
-    <sheet name="Add Bank" sheetId="3" r:id="rId10"/>
-    <sheet name="Verification Company" sheetId="4" r:id="rId11"/>
+    <sheet name="Connect Account" sheetId="14" r:id="rId3"/>
+    <sheet name="Create Stripe Account" sheetId="15" r:id="rId4"/>
+    <sheet name="Check Company Account " sheetId="5" r:id="rId5"/>
+    <sheet name="My Company" sheetId="6" r:id="rId6"/>
+    <sheet name="List DeletedCompany" sheetId="9" r:id="rId7"/>
+    <sheet name="Update Company" sheetId="12" r:id="rId8"/>
+    <sheet name="Create Compan" sheetId="13" r:id="rId9"/>
+    <sheet name="Detail Company" sheetId="10" r:id="rId10"/>
+    <sheet name="Group of CompanyID" sheetId="11" r:id="rId11"/>
+    <sheet name="Add Bank" sheetId="3" r:id="rId12"/>
+    <sheet name="Verification Company" sheetId="4" r:id="rId13"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="201">
   <si>
     <t>TestCase-SeekProductAPI</t>
   </si>
@@ -195,130 +197,6 @@
   </si>
   <si>
     <t>{
-    "id": "acct_1HFIzxC4KWdFBXYf",
-    "object": "account",
-    "business_logo": null,
-    "business_logo_large": null,
-    "business_name": "PC",
-    "business_primary_color": null,
-    "business_url": null,
-    "capabilities": {
-        "legacy_payments": "active"
-    },
-    "charges_enabled": true,
-    "country": "AU",
-    "created": 1597235045,
-    "debit_negative_balances": false,
-    "decline_charge_on": {
-        "avs_failure": false,
-        "cvc_failure": false
-    },
-    "default_currency": "aud",
-    "details_submitted": true,
-    "display_name": null,
-    "email": "admin@gmail.com",
-    "external_accounts": {
-        "object": "list",
-        "data": [
-            {
-                "id": "ba_1HGc4zC4KWdFBXYfXGsaKXcP",
-                "object": "bank_account",
-                "account": "acct_1HFIzxC4KWdFBXYf",
-                "account_holder_name": "Dave",
-                "account_holder_type": "company",
-                "bank_name": "STRIPE TEST BANK",
-                "country": "AU",
-                "currency": "aud",
-                "default_for_currency": true,
-                "fingerprint": "yk5SEpjbOehQvnza",
-                "last4": "3456",
-                "metadata": {},
-                "routing_number": "11 0000",
-                "status": "new"
-            }
-        ],
-        "has_more": false,
-        "total_count": 1,
-        "url": "/v1/accounts/acct_1HFIzxC4KWdFBXYf/external_accounts"
-    },
-    "legal_entity": {
-        "additional_owners": [],
-        "address": {
-            "city": "Texas",
-            "country": "AU",
-            "line1": "Texas",
-            "line2": null,
-            "postal_code": "2148",
-            "state": "NSW"
-        },
-        "business_name": "PC",
-        "business_tax_id_provided": true,
-        "directors_provided": false,
-        "dob": {
-            "day": 12,
-            "month": 12,
-            "year": 1984
-        },
-        "executives_provided": false,
-        "first_name": "ABC",
-        "last_name": "David",
-        "owners_provided": false,
-        "personal_address": {
-            "city": null,
-            "country": "AU",
-            "line1": null,
-            "line2": null,
-            "postal_code": null,
-            "state": null
-        },
-        "type": "company",
-        "verification": {
-            "additional_document": null,
-            "additional_document_back": null,
-            "details": null,
-            "details_code": null,
-            "document": "file_1HGc4zC4KWdFBXYf7NO6bBeU",
-            "document_back": null,
-            "status": "pending"
-        }
-    },
-    "mcc": null,
-    "metadata": {},
-    "payout_schedule": {
-        "delay_days": 2,
-        "interval": "daily"
-    },
-    "payout_statement_descriptor": null,
-    "payouts_enabled": true,
-    "product_description": null,
-    "statement_descriptor": "",
-    "statement_descriptor_kana": null,
-    "statement_descriptor_kanji": null,
-    "support_address": null,
-    "support_email": null,
-    "support_phone": null,
-    "support_url": null,
-    "timezone": "Etc/UTC",
-    "tos_acceptance": {
-        "date": 1597546722,
-        "ip": "8.8.8.8",
-        "user_agent": null
-    },
-    "type": "custom",
-    "verification": {
-        "disabled_reason": null,
-        "due_by": null,
-        "errors": [],
-        "fields_needed": [],
-        "pending_verification": []
-    }
-}</t>
-  </si>
-  <si>
-    <t>"error": "You cannot use a Stripe token more than once: btok_1HGc4pDyifgV66lTrbD7m1Ux."</t>
-  </si>
-  <si>
-    <t>{
     "id": 289,
     "user": 2,
     "store_name": "X1 Store",
@@ -345,130 +223,6 @@
     "status": "unverified",
     "is_subscribed": false,
     "social_status": false
-}</t>
-  </si>
-  <si>
-    <t>mỗi btok chỉ sử dụng để xác minh 1 company</t>
-  </si>
-  <si>
-    <t>{
-    "id": "acct_1HGcXsAzh19G0re1",
-    "object": "account",
-    "business_logo": null,
-    "business_logo_large": null,
-    "business_name": "PC",
-    "business_primary_color": null,
-    "business_url": null,
-    "capabilities": {
-        "legacy_payments": "active"
-    },
-    "charges_enabled": true,
-    "country": "AU",
-    "created": 1597548512,
-    "debit_negative_balances": false,
-    "decline_charge_on": {
-        "avs_failure": false,
-        "cvc_failure": false
-    },
-    "default_currency": "aud",
-    "details_submitted": true,
-    "display_name": null,
-    "email": "admin@gmail.com",
-    "external_accounts": {
-        "object": "list",
-        "data": [
-            {
-                "id": "ba_1HGcbtAzh19G0re12JOe9wsB",
-                "object": "bank_account",
-                "account": "acct_1HGcXsAzh19G0re1",
-                "account_holder_name": "Dave",
-                "account_holder_type": "company",
-                "bank_name": "STRIPE TEST BANK",
-                "country": "AU",
-                "currency": "aud",
-                "default_for_currency": true,
-                "fingerprint": "yk5SEpjbOehQvnza",
-                "last4": "3456",
-                "metadata": {},
-                "routing_number": "11 0000",
-                "status": "new"
-            }
-        ],
-        "has_more": false,
-        "total_count": 1,
-        "url": "/v1/accounts/acct_1HGcXsAzh19G0re1/external_accounts"
-    },
-    "legal_entity": {
-        "additional_owners": [],
-        "address": {
-            "city": "Texas",
-            "country": "AU",
-            "line1": "Texas",
-            "line2": null,
-            "postal_code": "2148",
-            "state": "NSW"
-        },
-        "business_name": "PC",
-        "business_tax_id_provided": true,
-        "directors_provided": false,
-        "dob": {
-            "day": 12,
-            "month": 12,
-            "year": 1984
-        },
-        "executives_provided": false,
-        "first_name": "ABC",
-        "last_name": "David",
-        "owners_provided": false,
-        "personal_address": {
-            "city": null,
-            "country": "AU",
-            "line1": null,
-            "line2": null,
-            "postal_code": null,
-            "state": null
-        },
-        "type": "company",
-        "verification": {
-            "additional_document": null,
-            "additional_document_back": null,
-            "details": null,
-            "details_code": null,
-            "document": "file_1HGcbtAzh19G0re1Uw321FFw",
-            "document_back": null,
-            "status": "pending"
-        }
-    },
-    "mcc": null,
-    "metadata": {},
-    "payout_schedule": {
-        "delay_days": 2,
-        "interval": "daily"
-    },
-    "payout_statement_descriptor": null,
-    "payouts_enabled": true,
-    "product_description": null,
-    "statement_descriptor": "",
-    "statement_descriptor_kana": null,
-    "statement_descriptor_kanji": null,
-    "support_address": null,
-    "support_email": null,
-    "support_phone": null,
-    "support_url": null,
-    "timezone": "Etc/UTC",
-    "tos_acceptance": {
-        "date": 1597548762,
-        "ip": "8.8.8.8",
-        "user_agent": null
-    },
-    "type": "custom",
-    "verification": {
-        "disabled_reason": null,
-        "due_by": null,
-        "errors": [],
-        "fields_needed": [],
-        "pending_verification": []
-    }
 }</t>
   </si>
   <si>
@@ -2604,6 +2358,442 @@
   </si>
   <si>
     <t>banner="C:/image/a.jpg"                         logo="C:/image/a.jpg"                                   ad_sample="C:/image/a.jpj"</t>
+  </si>
+  <si>
+    <t>Connect Account</t>
+  </si>
+  <si>
+    <t>TC1_Seek_ConnectAccount</t>
+  </si>
+  <si>
+    <t>TC2_Seek_ConnectAccount</t>
+  </si>
+  <si>
+    <t>TC3_Seek_ConnectAccount</t>
+  </si>
+  <si>
+    <r>
+      <t>Connect Account with logged in &amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> valid token</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Connect Account with logged in &amp; invalid </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>token</t>
+    </r>
+  </si>
+  <si>
+    <t>Connect Account with logged in &amp; token has expired</t>
+  </si>
+  <si>
+    <t>Message: "https://connect.stripe.com/oauth/authorize?scope=read_write&amp;client_id=ca_DSoDpWXBCA8Q4nGiMyrT0ARtOXI0rSK9&amp;response_type=code"</t>
+  </si>
+  <si>
+    <t>Create Stripe Account</t>
+  </si>
+  <si>
+    <t>TC1_Seek_CreateStripeAccount</t>
+  </si>
+  <si>
+    <r>
+      <t>Create Stripe Account with logged in &amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> valid token</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create Stripe Account with logged in &amp; invalid </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>token</t>
+    </r>
+  </si>
+  <si>
+    <t>Create Stripe Account with logged in &amp; token has expired</t>
+  </si>
+  <si>
+    <t>Message: "photo_id_front": 
+        "The submitted data was not a file. Check the encoding type on the form."</t>
+  </si>
+  <si>
+    <t>Verification Company</t>
+  </si>
+  <si>
+    <t>TC1_Seek_VerificationCompany</t>
+  </si>
+  <si>
+    <t>TC2_Seek_VerificationCompany</t>
+  </si>
+  <si>
+    <t>TC3_Seek_VerificationCompany</t>
+  </si>
+  <si>
+    <t>TC4_Seek_VerificationCompany</t>
+  </si>
+  <si>
+    <r>
+      <t>Create Stripe Account with logged in &amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> valid token &amp; photo_id_front </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>is invalid</t>
+    </r>
+  </si>
+  <si>
+    <t>photo_id_front = "xxx"</t>
+  </si>
+  <si>
+    <r>
+      <t>Create Stripe Account with logged in &amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> valid token &amp; bank_token </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>is invalid</t>
+    </r>
+  </si>
+  <si>
+    <t>bank_token ="xxxx"</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Account logged in &amp; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>invalid bank_token</t>
+    </r>
+  </si>
+  <si>
+    <t>Account logged in &amp; invalid photo_id_front</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Message: "Unauthorized"</t>
+  </si>
+  <si>
+    <r>
+      <t>Create Stripe Account with logged in &amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> valid all fields property</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Account logged in &amp; valid </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">all fields property  </t>
+    </r>
+  </si>
+  <si>
+    <t>Message:{
+    "id": "acct_1HGlj4IRuvBs8zdB",
+    "object": "account",
+    "business_logo": null,
+    "business_logo_large": null,
+    "business_name": "PC",
+    "business_primary_color": null,
+    "business_url": null,
+    "capabilities": {
+        "legacy_payments": "active"
+    },
+    "charges_enabled": true,
+    "country": "AU",
+    "created": 1597583803,
+    "debit_negative_balances": false,
+    "decline_charge_on": {
+        "avs_failure": false,
+        "cvc_failure": false
+    },
+    "default_currency": "aud",
+    "details_submitted": true,
+    "display_name": null,
+    "email": "phucsteam98@gmail.com",
+    "external_accounts": {
+        "object": "list",
+        "data": [
+            {
+                "id": "ba_1HJEr2IRuvBs8zdBZegYaGPr",
+                "object": "bank_account",
+                "account": "acct_1HGlj4IRuvBs8zdB",
+                "account_holder_name": "Dave",
+                "account_holder_type": "company",
+                "bank_name": "STRIPE TEST BANK",
+                "country": "AU",
+                "currency": "aud",
+                "default_for_currency": true,
+                "fingerprint": "yk5SEpjbOehQvnza",
+                "last4": "3456",
+                "metadata": {},
+                "routing_number": "11 0000",
+                "status": "new"
+            }
+        ],
+        "has_more": false,
+        "total_count": 1,
+        "url": "/v1/accounts/acct_1HGlj4IRuvBs8zdB/external_accounts"
+    },
+    "legal_entity": {
+        "additional_owners": [],
+        "address": {
+            "city": "Texas",
+            "country": "AU",
+            "line1": "Texas",
+            "line2": null,
+            "postal_code": "2148",
+            "state": "NSW"
+        },
+        "business_name": "PC",
+        "business_tax_id_provided": true,
+        "directors_provided": false,
+        "dob": {
+            "day": 12,
+            "month": 12,
+            "year": 1984
+        },
+        "executives_provided": false,
+        "first_name": "ABC",
+        "last_name": "David",
+        "owners_provided": false,
+        "personal_address": {
+            "city": null,
+            "country": "AU",
+            "line1": null,
+            "line2": null,
+            "postal_code": null,
+            "state": null
+        },
+        "type": "company",
+        "verification": {
+            "additional_document": null,
+            "additional_document_back": null,
+            "details": null,
+            "details_code": null,
+            "document": "file_1HJEr2IRuvBs8zdBmjxcgNaW",
+            "document_back": null,
+            "status": "pending"
+        }
+    },
+    "mcc": null,
+    "metadata": {},
+    "payout_schedule": {
+        "delay_days": 2,
+        "interval": "daily"
+    },
+    "payout_statement_descriptor": null,
+    "payouts_enabled": true,
+    "product_description": null,
+    "statement_descriptor": "",
+    "statement_descriptor_kana": null,
+    "statement_descriptor_kanji": null,
+    "support_address": null,
+    "support_email": null,
+    "support_phone": null,
+    "support_url": null,
+    "timezone": "Etc/UTC",
+    "tos_acceptance": {
+        "date": 1598172429,
+        "ip": "8.8.8.8",
+        "user_agent": null
+    },
+    "type": "custom",
+    "verification": {
+        "disabled_reason": null,
+        "due_by": null,
+        "errors": [],
+        "fields_needed": [],
+        "pending_verification": []
+    }
+}</t>
+  </si>
+  <si>
+    <r>
+      <t>Create Stripe Account with logged in &amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> valid token &amp; bank_token </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>has been used already</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Account logged in &amp; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>bank_token has been used already</t>
+    </r>
+  </si>
+  <si>
+    <t>bank_token ="btok_1HJEpnDyifgV66lTZZGNV9CV"</t>
+  </si>
+  <si>
+    <t>Message: "error": "You cannot use a Stripe token more than once: btok_1HJEpnDyifgV66lTZZGNV9CV."</t>
+  </si>
+  <si>
+    <t>Message:"error": "You cannot change `legal_entity[verification][document]` via API if an account is verified. Please contact us via https://support.stripe.com/contact if you need to change the legal entity information associated with this account.""</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create Stripe Account with logged in &amp; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>account</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> already verified</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Account logged in &amp; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>account already verified</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -3020,7 +3210,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3160,6 +3350,334 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="36" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28" customWidth="1"/>
+    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="240" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" ht="96.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:J15"/>
   <sheetViews>
@@ -3197,7 +3715,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -3242,22 +3760,22 @@
     </row>
     <row r="7" spans="1:10" ht="115.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>47</v>
-      </c>
       <c r="E7" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>16</v>
@@ -3270,22 +3788,22 @@
     </row>
     <row r="8" spans="1:10" ht="78" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>16</v>
@@ -3298,22 +3816,22 @@
     </row>
     <row r="9" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>16</v>
@@ -3332,41 +3850,281 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="H7:I10"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="36.44140625" customWidth="1"/>
     <col min="9" max="9" width="49.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="8:9" ht="16.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="I8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="8:9" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H9" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="8:9" ht="69" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I10" t="s">
-        <v>37</v>
-      </c>
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="36" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="1:10" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+    </row>
+    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F14" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3374,7 +4132,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -3458,11 +4216,11 @@
         <v>30</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>32</v>
@@ -3481,17 +4239,17 @@
         <v>29</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>16</v>
@@ -3507,17 +4265,17 @@
         <v>29</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>16</v>
@@ -3533,17 +4291,17 @@
         <v>29</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>16</v>
@@ -3559,17 +4317,17 @@
         <v>29</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>16</v>
@@ -3585,19 +4343,19 @@
         <v>29</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>16</v>
@@ -3613,19 +4371,19 @@
         <v>29</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>31</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>33</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>16</v>
@@ -3641,19 +4399,19 @@
         <v>29</v>
       </c>
       <c r="B14" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>168</v>
-      </c>
       <c r="E14" s="5" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>16</v>
@@ -3675,7 +4433,7 @@
     </row>
     <row r="36" spans="6:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="F36" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>28</v>
@@ -3691,6 +4449,335 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D227C71F-EA37-41F5-8D2A-33B84880E086}">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J9" sqref="A1:J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.44140625" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="36" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93F1D4AB-B47A-4EDF-B980-4B2CEA220DA3}">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J9" sqref="A1:J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.5546875" customWidth="1"/>
+    <col min="7" max="7" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="36" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="131.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J12"/>
   <sheetViews>
@@ -3727,7 +4814,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -3772,22 +4859,22 @@
     </row>
     <row r="7" spans="1:10" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="D7" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>16</v>
@@ -3800,22 +4887,22 @@
     </row>
     <row r="8" spans="1:10" ht="87" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>16</v>
@@ -3828,22 +4915,22 @@
     </row>
     <row r="9" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>16</v>
@@ -3856,22 +4943,22 @@
     </row>
     <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>61</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>16</v>
@@ -3884,20 +4971,20 @@
     </row>
     <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>16</v>
@@ -3917,12 +5004,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3957,7 +5044,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -4002,20 +5089,20 @@
     </row>
     <row r="7" spans="1:10" ht="129.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>101</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>16</v>
@@ -4028,20 +5115,20 @@
     </row>
     <row r="8" spans="1:10" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>16</v>
@@ -4054,20 +5141,20 @@
     </row>
     <row r="9" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>16</v>
@@ -4106,12 +5193,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="A1:J9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4146,7 +5233,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -4191,20 +5278,20 @@
     </row>
     <row r="7" spans="1:10" ht="96.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>16</v>
@@ -4217,20 +5304,20 @@
     </row>
     <row r="8" spans="1:10" ht="94.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>16</v>
@@ -4243,20 +5330,20 @@
     </row>
     <row r="9" spans="1:10" ht="89.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>16</v>
@@ -4272,7 +5359,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:M19"/>
   <sheetViews>
@@ -4314,7 +5401,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -4359,20 +5446,20 @@
     </row>
     <row r="7" spans="1:10" ht="133.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>16</v>
@@ -4385,20 +5472,20 @@
     </row>
     <row r="8" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>16</v>
@@ -4411,20 +5498,20 @@
     </row>
     <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>16</v>
@@ -4437,20 +5524,20 @@
     </row>
     <row r="10" spans="1:10" ht="205.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>16</v>
@@ -4463,22 +5550,22 @@
     </row>
     <row r="11" spans="1:10" ht="109.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>16</v>
@@ -4491,22 +5578,22 @@
     </row>
     <row r="12" spans="1:10" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>16</v>
@@ -4519,22 +5606,22 @@
     </row>
     <row r="13" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>16</v>
@@ -4547,22 +5634,22 @@
     </row>
     <row r="14" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>16</v>
@@ -4578,7 +5665,7 @@
     </row>
     <row r="19" spans="13:13" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M19" s="8" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -4587,7 +5674,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="M23:M24"/>
   <sheetViews>
@@ -4602,341 +5689,13 @@
   <sheetData>
     <row r="23" spans="13:13" ht="249.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M23" s="8" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="24" spans="13:13" ht="186.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M24" s="8" t="s">
-        <v>157</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:J9"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="36" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-    </row>
-    <row r="8" spans="1:10" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-    </row>
-    <row r="9" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:J9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28" customWidth="1"/>
-    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="240" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-    </row>
-    <row r="8" spans="1:10" ht="96.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-    </row>
-    <row r="9" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
+        <v>153</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#phuc.nguyen update Company & update banner
</commit_message>
<xml_diff>
--- a/docs/HuuPhuc/Manager Company 1.xlsx
+++ b/docs/HuuPhuc/Manager Company 1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41DDA297-660D-4691-A781-DC8982DF4748}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E983DF3-8B05-4588-A652-EB29BF0D196F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All My Company" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,8 @@
     <sheet name="Detail Company" sheetId="10" r:id="rId10"/>
     <sheet name="Group of CompanyID" sheetId="11" r:id="rId11"/>
     <sheet name="Add Bank" sheetId="3" r:id="rId12"/>
-    <sheet name="Verification Company" sheetId="4" r:id="rId13"/>
+    <sheet name="Add Social Link" sheetId="16" r:id="rId13"/>
+    <sheet name="Verification Company" sheetId="4" r:id="rId14"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="217">
   <si>
     <t>TestCase-SeekProductAPI</t>
   </si>
@@ -2795,12 +2796,208 @@
       <t>account already verified</t>
     </r>
   </si>
+  <si>
+    <t>Add Social Link</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Add Social Link with logged in &amp; invalid </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>token</t>
+    </r>
+  </si>
+  <si>
+    <t>Add Social Link with logged in &amp; token has expired</t>
+  </si>
+  <si>
+    <t>TC1_Seek_AddSocialLink</t>
+  </si>
+  <si>
+    <t>TC2_Seek_AddSocialLink</t>
+  </si>
+  <si>
+    <t>TC3_Seek_AddSocialLink</t>
+  </si>
+  <si>
+    <t>TC4_Seek_AddSocialLink</t>
+  </si>
+  <si>
+    <r>
+      <t>Add Social Link with logged in &amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> valid token </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">&amp; valid </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>id_company</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &amp; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>company</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from the up silver up</t>
+    </r>
+  </si>
+  <si>
+    <t>Message :{
+    "facebook": "facebook.com/itech/",
+    "instagram": "instagram.com/itech/",
+    "twitter": "twitter.com/itech/"
+}</t>
+  </si>
+  <si>
+    <t>A message   "You need Silver subscription to add socail links"</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Account logged in &amp; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>valid token  &amp; valid id_company &amp; company from the up silver up</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Add Social Link with logged in &amp; token valid </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">token  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&amp; company unregistered subscription</t>
+    </r>
+  </si>
+  <si>
+    <t>data : {
+ "facebook":"facebook.com/itech/",
+ "instagram":"instagram.com/itech/",
+ "twitter":"twitter.com/itech/"
+}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Add Social Link with logged in &amp; invalid </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>company_id</t>
+    </r>
+  </si>
+  <si>
+    <t>A message   "company": "not found"</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Account logged in   &amp; invalid </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>company_id</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3213,7 +3410,7 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
@@ -3227,12 +3424,12 @@
     <col min="10" max="10" width="9.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="21">
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -3240,7 +3437,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -3248,7 +3445,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -3256,7 +3453,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="18">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -3288,7 +3485,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="107.4" customHeight="1">
       <c r="A7" s="6" t="s">
         <v>18</v>
       </c>
@@ -3316,7 +3513,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="1:10" ht="81" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="81" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>18</v>
       </c>
@@ -3357,7 +3554,7 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.44140625" bestFit="1" customWidth="1"/>
@@ -3369,12 +3566,12 @@
     <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="21">
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -3382,7 +3579,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -3390,7 +3587,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -3398,7 +3595,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="36" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="36">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -3430,7 +3627,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="77.400000000000006" customHeight="1">
       <c r="A7" s="6" t="s">
         <v>107</v>
       </c>
@@ -3456,7 +3653,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="1:10" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="57.6" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>107</v>
       </c>
@@ -3482,7 +3679,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="72">
       <c r="A9" s="6" t="s">
         <v>107</v>
       </c>
@@ -3519,10 +3716,10 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
@@ -3533,12 +3730,12 @@
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="21">
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -3546,7 +3743,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -3554,7 +3751,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -3562,7 +3759,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="18">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -3594,7 +3791,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="240" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="240" customHeight="1">
       <c r="A7" s="6" t="s">
         <v>114</v>
       </c>
@@ -3620,7 +3817,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="1:10" ht="96.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="96.6" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>114</v>
       </c>
@@ -3646,7 +3843,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="72">
       <c r="A9" s="6" t="s">
         <v>114</v>
       </c>
@@ -3681,11 +3878,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.44140625" bestFit="1" customWidth="1"/>
@@ -3697,12 +3894,12 @@
     <col min="10" max="10" width="32.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="21">
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -3710,7 +3907,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -3718,7 +3915,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -3726,7 +3923,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="18">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -3758,7 +3955,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="115.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="409.6">
       <c r="A7" s="6" t="s">
         <v>35</v>
       </c>
@@ -3786,7 +3983,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="1:10" ht="78" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="78" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>35</v>
       </c>
@@ -3814,7 +4011,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="72">
       <c r="A9" s="6" t="s">
         <v>35</v>
       </c>
@@ -3842,7 +4039,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10">
       <c r="J15" s="9"/>
     </row>
   </sheetData>
@@ -3851,14 +4048,233 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62E0C768-918A-4BA7-B4DA-DF4A9A451050}">
+  <dimension ref="A1:P11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="28" customWidth="1"/>
+    <col min="8" max="8" width="15.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="21">
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="18">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="116.4" customHeight="1">
+      <c r="A7" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:16" ht="43.2">
+      <c r="A8" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:16" ht="57.6">
+      <c r="A9" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="P9" s="8"/>
+    </row>
+    <row r="10" spans="1:16" ht="100.8">
+      <c r="A10" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" spans="1:16" ht="57.6">
+      <c r="A11" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.21875" bestFit="1" customWidth="1"/>
@@ -3870,12 +4286,12 @@
     <col min="9" max="9" width="49.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="21">
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -3883,7 +4299,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -3891,7 +4307,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -3899,7 +4315,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="36" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="36">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -3931,7 +4347,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="72" customHeight="1">
       <c r="A7" s="6" t="s">
         <v>179</v>
       </c>
@@ -3957,7 +4373,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="72">
       <c r="A8" s="6" t="s">
         <v>179</v>
       </c>
@@ -3985,7 +4401,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="1:10" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="57" customHeight="1">
       <c r="A9" s="6" t="s">
         <v>179</v>
       </c>
@@ -4013,7 +4429,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
     </row>
-    <row r="10" spans="1:10" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="69" customHeight="1">
       <c r="A10" s="6" t="s">
         <v>179</v>
       </c>
@@ -4041,7 +4457,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
     </row>
-    <row r="11" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="129.6">
       <c r="A11" s="6" t="s">
         <v>179</v>
       </c>
@@ -4067,7 +4483,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
     </row>
-    <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="43.2">
       <c r="A12" s="6" t="s">
         <v>179</v>
       </c>
@@ -4093,7 +4509,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
     </row>
-    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="43.2">
       <c r="A13" s="6" t="s">
         <v>179</v>
       </c>
@@ -4119,7 +4535,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10">
       <c r="F14" s="8"/>
     </row>
   </sheetData>
@@ -4132,11 +4548,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
@@ -4147,12 +4563,12 @@
     <col min="7" max="7" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="21">
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -4160,7 +4576,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -4168,7 +4584,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -4176,7 +4592,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="20.399999999999999" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -4208,7 +4624,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="283.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="283.8" customHeight="1">
       <c r="A7" s="6" t="s">
         <v>29</v>
       </c>
@@ -4234,7 +4650,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="1:10" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="48.6" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>29</v>
       </c>
@@ -4260,7 +4676,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="57.6">
       <c r="A9" s="6" t="s">
         <v>29</v>
       </c>
@@ -4286,7 +4702,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
     </row>
-    <row r="10" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="57.6">
       <c r="A10" s="6" t="s">
         <v>29</v>
       </c>
@@ -4312,7 +4728,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
     </row>
-    <row r="11" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="57.6">
       <c r="A11" s="6" t="s">
         <v>29</v>
       </c>
@@ -4338,7 +4754,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
     </row>
-    <row r="12" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="72">
       <c r="A12" s="6" t="s">
         <v>29</v>
       </c>
@@ -4366,7 +4782,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
     </row>
-    <row r="13" spans="1:10" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="70.2" customHeight="1">
       <c r="A13" s="6" t="s">
         <v>29</v>
       </c>
@@ -4394,7 +4810,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
     </row>
-    <row r="14" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="115.2">
       <c r="A14" s="6" t="s">
         <v>29</v>
       </c>
@@ -4422,16 +4838,16 @@
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10">
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10">
       <c r="G16" s="8"/>
     </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="6:6">
       <c r="F20" s="8"/>
     </row>
-    <row r="36" spans="6:7" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="6:7" ht="409.6">
       <c r="F36" s="8" t="s">
         <v>34</v>
       </c>
@@ -4439,7 +4855,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="6:7">
       <c r="F41" s="8"/>
     </row>
   </sheetData>
@@ -4456,7 +4872,7 @@
       <selection activeCell="J9" sqref="A1:J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.109375" bestFit="1" customWidth="1"/>
@@ -4469,12 +4885,12 @@
     <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="21">
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -4482,7 +4898,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -4490,7 +4906,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -4498,7 +4914,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="36" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="36">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -4530,7 +4946,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="104.4" customHeight="1">
       <c r="A7" s="6" t="s">
         <v>165</v>
       </c>
@@ -4556,7 +4972,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="43.2">
       <c r="A8" s="6" t="s">
         <v>165</v>
       </c>
@@ -4582,7 +4998,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="57.6">
       <c r="A9" s="6" t="s">
         <v>165</v>
       </c>
@@ -4618,10 +5034,10 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="J9" sqref="A1:J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
@@ -4633,12 +5049,12 @@
     <col min="8" max="8" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="21">
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -4646,7 +5062,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -4654,7 +5070,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -4662,7 +5078,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="36" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="36">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -4694,7 +5110,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="131.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="131.4" customHeight="1">
       <c r="A7" s="6" t="s">
         <v>173</v>
       </c>
@@ -4720,7 +5136,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="57.6">
       <c r="A8" s="6" t="s">
         <v>173</v>
       </c>
@@ -4746,7 +5162,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="57.6">
       <c r="A9" s="6" t="s">
         <v>173</v>
       </c>
@@ -4785,7 +5201,7 @@
       <selection activeCell="G11" sqref="F10:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="22.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.44140625" bestFit="1" customWidth="1"/>
@@ -4796,12 +5212,12 @@
     <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="21">
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -4809,7 +5225,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -4817,7 +5233,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -4825,7 +5241,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="18">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -4857,7 +5273,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="69" customHeight="1">
       <c r="A7" s="6" t="s">
         <v>53</v>
       </c>
@@ -4885,7 +5301,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="1:10" ht="87" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="87" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>53</v>
       </c>
@@ -4913,7 +5329,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="48" customHeight="1">
       <c r="A9" s="6" t="s">
         <v>53</v>
       </c>
@@ -4941,7 +5357,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
     </row>
-    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="28.8">
       <c r="A10" s="6" t="s">
         <v>53</v>
       </c>
@@ -4969,7 +5385,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
     </row>
-    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="28.8">
       <c r="A11" s="6" t="s">
         <v>53</v>
       </c>
@@ -4995,7 +5411,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10">
       <c r="F12" s="10"/>
     </row>
   </sheetData>
@@ -5012,7 +5428,7 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="21.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.109375" bestFit="1" customWidth="1"/>
@@ -5026,12 +5442,12 @@
     <col min="10" max="10" width="9.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="21">
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -5039,7 +5455,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -5047,7 +5463,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -5055,7 +5471,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="18">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -5087,7 +5503,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="129.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="129.6" customHeight="1">
       <c r="A7" s="6" t="s">
         <v>93</v>
       </c>
@@ -5113,7 +5529,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="1:10" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="48.6" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>93</v>
       </c>
@@ -5139,7 +5555,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="72">
       <c r="A9" s="6" t="s">
         <v>93</v>
       </c>
@@ -5165,7 +5581,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
     </row>
-    <row r="10" spans="1:10" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="64.8" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="12"/>
@@ -5176,7 +5592,7 @@
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
     </row>
-    <row r="11" spans="1:10" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="46.8" customHeight="1">
       <c r="A11" s="11"/>
       <c r="B11" s="11"/>
       <c r="C11" s="12"/>
@@ -5201,7 +5617,7 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="22.21875" customWidth="1"/>
     <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
@@ -5215,12 +5631,12 @@
     <col min="10" max="10" width="9.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="21">
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -5228,7 +5644,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -5236,7 +5652,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -5244,7 +5660,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="18">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -5276,7 +5692,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="96.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="96.6" customHeight="1">
       <c r="A7" s="6" t="s">
         <v>103</v>
       </c>
@@ -5302,7 +5718,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="1:10" ht="94.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="94.8" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>103</v>
       </c>
@@ -5328,7 +5744,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="1:10" ht="89.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="89.4" customHeight="1">
       <c r="A9" s="6" t="s">
         <v>103</v>
       </c>
@@ -5367,7 +5783,7 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.77734375" bestFit="1" customWidth="1"/>
@@ -5383,12 +5799,12 @@
     <col min="13" max="13" width="36.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="21">
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -5396,7 +5812,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -5404,7 +5820,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -5412,7 +5828,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="18">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -5444,7 +5860,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="133.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="133.19999999999999" customHeight="1">
       <c r="A7" s="6" t="s">
         <v>103</v>
       </c>
@@ -5470,7 +5886,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="43.2">
       <c r="A8" s="6" t="s">
         <v>103</v>
       </c>
@@ -5496,7 +5912,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="43.2">
       <c r="A9" s="6" t="s">
         <v>103</v>
       </c>
@@ -5522,7 +5938,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
     </row>
-    <row r="10" spans="1:10" ht="205.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="205.8" customHeight="1">
       <c r="A10" s="6" t="s">
         <v>103</v>
       </c>
@@ -5548,7 +5964,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
     </row>
-    <row r="11" spans="1:10" ht="109.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="109.2" customHeight="1">
       <c r="A11" s="6" t="s">
         <v>103</v>
       </c>
@@ -5576,7 +5992,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
     </row>
-    <row r="12" spans="1:10" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="83.4" customHeight="1">
       <c r="A12" s="6" t="s">
         <v>103</v>
       </c>
@@ -5604,7 +6020,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
     </row>
-    <row r="13" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="57.6">
       <c r="A13" s="6" t="s">
         <v>103</v>
       </c>
@@ -5632,7 +6048,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
     </row>
-    <row r="14" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="57.6">
       <c r="A14" s="6" t="s">
         <v>103</v>
       </c>
@@ -5660,10 +6076,10 @@
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10">
       <c r="F16" s="10"/>
     </row>
-    <row r="19" spans="13:13" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="13:13" ht="48.6" customHeight="1">
       <c r="M19" s="8" t="s">
         <v>133</v>
       </c>
@@ -5678,21 +6094,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="M23:M24"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="13" max="13" width="37.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="23" spans="13:13" ht="249.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="13:13" ht="249.6" customHeight="1">
       <c r="M23" s="8" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="24" spans="13:13" ht="186.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="13:13" ht="186.6" customHeight="1">
       <c r="M24" s="8" t="s">
         <v>153</v>
       </c>

</xml_diff>